<commit_message>
pnl, bs, cf are generated in excel through /routes
</commit_message>
<xml_diff>
--- a/pnl_excel/pnl_report.xlsx
+++ b/pnl_excel/pnl_report.xlsx
@@ -500,7 +500,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>330,858.46</t>
+          <t>7,677,623.38</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -522,7 +522,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>6,457,341.36</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -540,7 +540,7 @@
       <c r="B6" s="3" t="inlineStr"/>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>6,788,199.82</t>
+          <t>7,677,623.38</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>240,589.15</t>
+          <t>2,498.09</t>
         </is>
       </c>
       <c r="D8" s="5" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>63,394,867.00</t>
+          <t>63,498,614.00</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>203,329,874.72</t>
+          <t>215,212,520.99</t>
         </is>
       </c>
       <c r="D10" s="5" t="inlineStr">
@@ -638,12 +638,12 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
           <t>60,344,362.00</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>310,033.53</t>
+          <t>10,242,315.65</t>
         </is>
       </c>
       <c r="D13" s="5" t="inlineStr">
@@ -722,12 +722,12 @@
       <c r="B15" s="5" t="inlineStr"/>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>327,619,726.40</t>
+          <t>288,955,948.73</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>60,344,362.00</t>
         </is>
       </c>
     </row>
@@ -740,12 +740,12 @@
       <c r="B16" s="3" t="inlineStr"/>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>-320,831,526.58</t>
+          <t>-281,278,325.35</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-60,344,362.00</t>
         </is>
       </c>
     </row>
@@ -780,12 +780,12 @@
       <c r="B18" s="3" t="inlineStr"/>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>-320,831,526.58</t>
+          <t>-281,278,325.35</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-60,344,362.00</t>
         </is>
       </c>
     </row>
@@ -852,12 +852,12 @@
       <c r="B22" s="3" t="inlineStr"/>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>-320,831,526.58</t>
+          <t>-281,278,325.35</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-60,344,362.00</t>
         </is>
       </c>
     </row>

</xml_diff>